<commit_message>
WishList Test,Product comparison test cases implemented
</commit_message>
<xml_diff>
--- a/AutomationPractice/src/main/java/com/automationpractice/qa/testdata/AutomationPracticeTestData.xlsx
+++ b/AutomationPractice/src/main/java/com/automationpractice/qa/testdata/AutomationPracticeTestData.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15240" windowHeight="5520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14565" windowHeight="5520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" sheetId="1" r:id="rId1"/>
-    <sheet name="deals" sheetId="2" r:id="rId2"/>
+    <sheet name="products" sheetId="2" r:id="rId2"/>
     <sheet name="tasks" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1:I16"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>title</t>
   </si>
@@ -145,6 +146,30 @@
   </si>
   <si>
     <t>10/2/2002</t>
+  </si>
+  <si>
+    <t>srno</t>
+  </si>
+  <si>
+    <t>productCategory</t>
+  </si>
+  <si>
+    <t>productSubCategory</t>
+  </si>
+  <si>
+    <t>productName</t>
+  </si>
+  <si>
+    <t>quantity</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Dresses</t>
+  </si>
+  <si>
+    <t>Summer Dresses</t>
   </si>
 </sst>
 </file>
@@ -197,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -205,17 +230,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -496,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -655,12 +696,51 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="21.375" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>